<commit_message>
Inserimento Valutazioni Settimana 18/11/22
Co-Authored-By: Raffaele Squillante <75779944+Mr-Rafo@users.noreply.github.com>
Co-Authored-By: Antonio Giametta <58905671+AnttGiam@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/Documenti/Valutazioni/Valutazioni GreenLeaf.xlsx
+++ b/Documenti/Valutazioni/Valutazioni GreenLeaf.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\Desktop\Green-Leaf\Documenti\Valutazioni\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BED13326-23F0-4406-93F2-DF57715DA3FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AF63F405-AB08-4751-8B30-75669944DC3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" tabRatio="512" firstSheet="4" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13155" tabRatio="512" firstSheet="2" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Legenda" sheetId="1" r:id="rId1"/>
@@ -546,33 +546,22 @@
     <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -580,15 +569,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -609,31 +589,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Colore 1" xfId="1" builtinId="29"/>
@@ -641,19 +641,7 @@
   </cellStyles>
   <dxfs count="50">
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -692,13 +680,16 @@
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
@@ -711,6 +702,18 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
     </dxf>
     <dxf>
       <font>
@@ -845,9 +848,6 @@
       </font>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
       <font>
         <b/>
       </font>
@@ -1023,7 +1023,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1116,7 +1116,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1209,7 +1209,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1302,7 +1302,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1395,7 +1395,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1488,7 +1488,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>8.8000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -1965,7 +1965,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -2058,7 +2058,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -2151,7 +2151,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -2244,7 +2244,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -2337,7 +2337,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -2430,7 +2430,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>9.4</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -2907,7 +2907,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -3000,7 +3000,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -3093,7 +3093,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -3186,7 +3186,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -3279,7 +3279,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -3372,7 +3372,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>9.8000000000000007</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -3849,7 +3849,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -3942,7 +3942,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -4035,7 +4035,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -4128,7 +4128,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -4221,7 +4221,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -4314,7 +4314,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>9.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -4791,7 +4791,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -4884,7 +4884,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -4977,7 +4977,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>9</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -5070,7 +5070,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -5163,7 +5163,7 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -5256,7 +5256,7 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>9.6</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0</c:v>
@@ -8537,10 +8537,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{F406FB90-C344-4BD8-B912-818DEFD1A42C}" name="Tabella6812" displayName="Tabella6812" ref="A38:G43" totalsRowShown="0">
   <autoFilter ref="A38:G43" xr:uid="{F406FB90-C344-4BD8-B912-818DEFD1A42C}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{352DFAF2-91FD-4358-9272-9234D5167951}" name="Data" dataDxfId="3" totalsRowDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{F14240E8-70C5-4743-9D5A-8AE67D04D61F}" name="Proattività" dataDxfId="2">
-      <calculatedColumnFormula>'18-11-2022'!C7</calculatedColumnFormula>
-    </tableColumn>
+    <tableColumn id="1" xr3:uid="{352DFAF2-91FD-4358-9272-9234D5167951}" name="Data" dataDxfId="5" totalsRowDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{F14240E8-70C5-4743-9D5A-8AE67D04D61F}" name="Proattività" dataDxfId="3"/>
     <tableColumn id="3" xr3:uid="{2F833A7A-F703-420C-AD74-3DE18798A002}" name="Partecipazione">
       <calculatedColumnFormula>'18-11-2022'!D7</calculatedColumnFormula>
     </tableColumn>
@@ -8553,7 +8551,7 @@
     <tableColumn id="6" xr3:uid="{3B0F8CD7-37E4-435E-A587-E071658D4792}" name="Rispetto">
       <calculatedColumnFormula>'18-11-2022'!G7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{A87FA775-BA46-4890-A620-F208EBC658A9}" name="TOTALE" dataDxfId="0" totalsRowDxfId="1">
+    <tableColumn id="10" xr3:uid="{A87FA775-BA46-4890-A620-F208EBC658A9}" name="TOTALE" dataDxfId="2" totalsRowDxfId="1">
       <calculatedColumnFormula xml:space="preserve"> SUM(B39, C39, D39, E39, F39,) / 5</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -8562,13 +8560,13 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{98B2EC10-D7CB-4450-96FC-0D93FE538414}" name="Table2234523" displayName="Table2234523" ref="A2:I7" totalsRowShown="0" headerRowDxfId="43">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{98B2EC10-D7CB-4450-96FC-0D93FE538414}" name="Table2234523" displayName="Table2234523" ref="A2:I7" totalsRowShown="0" headerRowDxfId="44">
   <autoFilter ref="A2:I7" xr:uid="{8DC22752-3EC3-4188-AFEB-19590155F539}"/>
   <tableColumns count="9">
-    <tableColumn id="11" xr3:uid="{7705009F-014D-4F03-A168-362B71AF38A6}" name="Matricola" dataDxfId="42">
+    <tableColumn id="11" xr3:uid="{7705009F-014D-4F03-A168-362B71AF38A6}" name="Matricola" dataDxfId="43">
       <calculatedColumnFormula>Legenda!A2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{A8169774-1590-4C1C-9EF8-9C3EB925E46E}" name="Nome" dataDxfId="41">
+    <tableColumn id="1" xr3:uid="{A8169774-1590-4C1C-9EF8-9C3EB925E46E}" name="Nome" dataDxfId="42">
       <calculatedColumnFormula>CONCATENATE(Legenda!B2," ",Legenda!C2)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{D5AC2699-9764-4001-934B-8CD006D5FCF8}" name="Proattività"/>
@@ -8576,23 +8574,23 @@
     <tableColumn id="4" xr3:uid="{965734FB-4FE4-44C4-8149-BBDA87792EEA}" name="Qualità"/>
     <tableColumn id="5" xr3:uid="{5AA8B9A9-5029-4609-80B0-BFCF14B66732}" name="Relazioni"/>
     <tableColumn id="6" xr3:uid="{CBCF7E9B-A2A6-4F96-9E1E-6ECB4577ACB1}" name="Rispetto"/>
-    <tableColumn id="9" xr3:uid="{6A226AA0-A54D-4941-85AE-D3874652FDF4}" name="Voto calcolato" dataDxfId="40">
+    <tableColumn id="9" xr3:uid="{6A226AA0-A54D-4941-85AE-D3874652FDF4}" name="Voto calcolato" dataDxfId="41">
       <calculatedColumnFormula xml:space="preserve"> SUM(C3, D3, E3, F3, G3,#REF!,#REF!) / 7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{5BE36D1C-CF03-4FC2-AC25-5B9B390B44D3}" name="Voto Finale" dataDxfId="39"/>
+    <tableColumn id="10" xr3:uid="{5BE36D1C-CF03-4FC2-AC25-5B9B390B44D3}" name="Voto Finale" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4F89BB00-B709-4ED1-AA9C-BDBFE2FCBCA4}" name="Table22345234" displayName="Table22345234" ref="A2:I7" totalsRowShown="0" headerRowDxfId="38">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{4F89BB00-B709-4ED1-AA9C-BDBFE2FCBCA4}" name="Table22345234" displayName="Table22345234" ref="A2:I7" totalsRowShown="0" headerRowDxfId="39">
   <autoFilter ref="A2:I7" xr:uid="{8DC22752-3EC3-4188-AFEB-19590155F539}"/>
   <tableColumns count="9">
-    <tableColumn id="11" xr3:uid="{DDDE1589-7E98-47FC-8045-62949F21FB83}" name="Matricola" dataDxfId="37">
+    <tableColumn id="11" xr3:uid="{DDDE1589-7E98-47FC-8045-62949F21FB83}" name="Matricola" dataDxfId="38">
       <calculatedColumnFormula>Legenda!A2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{4CE25F92-ADBB-4C96-BDB1-11B47D348C7C}" name="Nome" dataDxfId="36">
+    <tableColumn id="1" xr3:uid="{4CE25F92-ADBB-4C96-BDB1-11B47D348C7C}" name="Nome" dataDxfId="37">
       <calculatedColumnFormula>CONCATENATE(Legenda!B2," ",Legenda!C2)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{5DC511BD-9B15-4842-9B58-708274E069B8}" name="Proattività"/>
@@ -8600,23 +8598,23 @@
     <tableColumn id="4" xr3:uid="{F85B8150-7B38-4A0E-B60E-5DE07DC76F40}" name="Qualità"/>
     <tableColumn id="5" xr3:uid="{106860A2-5062-4D49-835D-94FEE47002D2}" name="Relazioni"/>
     <tableColumn id="6" xr3:uid="{7A45FC28-4AA8-419F-BF4D-EA6EC77445F2}" name="Rispetto"/>
-    <tableColumn id="9" xr3:uid="{CDB36BDC-8104-40D4-A3CC-19CA95A0AC38}" name="Voto calcolato" dataDxfId="35">
+    <tableColumn id="9" xr3:uid="{CDB36BDC-8104-40D4-A3CC-19CA95A0AC38}" name="Voto calcolato" dataDxfId="36">
       <calculatedColumnFormula xml:space="preserve"> SUM(C3, D3, E3, F3, G3,#REF!,#REF!) / 7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{A461C54F-7C37-43BD-B853-F48C1404EF74}" name="Voto Finale" dataDxfId="34"/>
+    <tableColumn id="10" xr3:uid="{A461C54F-7C37-43BD-B853-F48C1404EF74}" name="Voto Finale" dataDxfId="35"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C2A4485E-8B68-4AB9-9B5A-02AC1E287945}" name="Table223452345" displayName="Table223452345" ref="A2:I7" totalsRowShown="0" headerRowDxfId="33">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{C2A4485E-8B68-4AB9-9B5A-02AC1E287945}" name="Table223452345" displayName="Table223452345" ref="A2:I7" totalsRowShown="0" headerRowDxfId="34">
   <autoFilter ref="A2:I7" xr:uid="{8DC22752-3EC3-4188-AFEB-19590155F539}"/>
   <tableColumns count="9">
-    <tableColumn id="11" xr3:uid="{6ACD335C-7F03-4C44-8C7E-8005A6404384}" name="Matricola" dataDxfId="32">
+    <tableColumn id="11" xr3:uid="{6ACD335C-7F03-4C44-8C7E-8005A6404384}" name="Matricola" dataDxfId="33">
       <calculatedColumnFormula>Legenda!A2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{5F054E26-7903-4DFE-A17E-2371E433E3D6}" name="Nome" dataDxfId="31">
+    <tableColumn id="1" xr3:uid="{5F054E26-7903-4DFE-A17E-2371E433E3D6}" name="Nome" dataDxfId="32">
       <calculatedColumnFormula>CONCATENATE(Legenda!B2," ",Legenda!C2)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{BC60AB95-6AA6-4C3A-A67F-E7460A1FC13E}" name="Proattività"/>
@@ -8624,23 +8622,23 @@
     <tableColumn id="4" xr3:uid="{4CEE8BCD-4851-40FD-93C9-1BFC493CB9CA}" name="Qualità"/>
     <tableColumn id="5" xr3:uid="{322A2791-5C29-4D6C-8428-675CD11029D1}" name="Relazioni"/>
     <tableColumn id="6" xr3:uid="{604653A8-5717-4F79-9D9B-27D3EB0903EE}" name="Rispetto"/>
-    <tableColumn id="9" xr3:uid="{F2DD7448-2987-4FEB-A560-8045D2BFD05C}" name="Voto calcolato" dataDxfId="30">
+    <tableColumn id="9" xr3:uid="{F2DD7448-2987-4FEB-A560-8045D2BFD05C}" name="Voto calcolato" dataDxfId="31">
       <calculatedColumnFormula xml:space="preserve"> SUM(C3, D3, E3, F3, G3,#REF!,#REF!) / 7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{C0FD815B-5F1C-49CE-B081-A75517B2D05A}" name="Voto Finale" dataDxfId="29"/>
+    <tableColumn id="10" xr3:uid="{C0FD815B-5F1C-49CE-B081-A75517B2D05A}" name="Voto Finale" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{4D6CBC9F-942C-44A1-8015-03D802B4EBAF}" name="Table2234523456" displayName="Table2234523456" ref="A2:I7" totalsRowShown="0" headerRowDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{4D6CBC9F-942C-44A1-8015-03D802B4EBAF}" name="Table2234523456" displayName="Table2234523456" ref="A2:I7" totalsRowShown="0" headerRowDxfId="29">
   <autoFilter ref="A2:I7" xr:uid="{8DC22752-3EC3-4188-AFEB-19590155F539}"/>
   <tableColumns count="9">
-    <tableColumn id="11" xr3:uid="{5019F27C-ECA1-47F6-8152-1B4A95AEEF3B}" name="Matricola" dataDxfId="27">
+    <tableColumn id="11" xr3:uid="{5019F27C-ECA1-47F6-8152-1B4A95AEEF3B}" name="Matricola" dataDxfId="28">
       <calculatedColumnFormula>Legenda!A2</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{F125D47E-FF92-4C45-ABCF-051BD2C4E6B9}" name="Nome" dataDxfId="26">
+    <tableColumn id="1" xr3:uid="{F125D47E-FF92-4C45-ABCF-051BD2C4E6B9}" name="Nome" dataDxfId="27">
       <calculatedColumnFormula>CONCATENATE(Legenda!B2," ",Legenda!C2)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="2" xr3:uid="{DB98E798-F9AB-46EB-AF4C-1AB7B6DC97FC}" name="Proattività"/>
@@ -8648,10 +8646,10 @@
     <tableColumn id="4" xr3:uid="{EA1AA272-A0DB-4AE7-9FC2-DDD9480E1DE8}" name="Qualità"/>
     <tableColumn id="5" xr3:uid="{4A8292BA-71AF-4108-9DFC-90834D546ED4}" name="Relazioni"/>
     <tableColumn id="6" xr3:uid="{EA1E0BA5-A356-4D8B-8214-69FC2B1E602A}" name="Rispetto"/>
-    <tableColumn id="9" xr3:uid="{1BD27B45-BA7B-4845-B4C4-97859C63831F}" name="Voto calcolato" dataDxfId="25">
+    <tableColumn id="9" xr3:uid="{1BD27B45-BA7B-4845-B4C4-97859C63831F}" name="Voto calcolato" dataDxfId="26">
       <calculatedColumnFormula xml:space="preserve"> SUM(C3, D3, E3, F3, G3,#REF!,#REF!) / 7</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{A1235308-CAD4-45B6-B87E-15B93D3ACDF4}" name="Voto Finale" dataDxfId="24"/>
+    <tableColumn id="10" xr3:uid="{A1235308-CAD4-45B6-B87E-15B93D3ACDF4}" name="Voto Finale" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium6" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -8661,15 +8659,15 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{5AE82BE7-A408-D144-A1FF-9EF6353C22D3}" name="Tabella68" displayName="Tabella68" ref="A2:G7" totalsRowShown="0">
   <autoFilter ref="A2:G7" xr:uid="{E0C560D8-06DD-E043-8D59-FEF48584D359}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{82F26A05-7812-994D-A732-53E6443686C3}" name="Data" dataDxfId="22" totalsRowDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{C0CE1913-F94A-6640-BCBC-B4DBAA74004F}" name="Proattività" dataDxfId="20">
+    <tableColumn id="1" xr3:uid="{82F26A05-7812-994D-A732-53E6443686C3}" name="Data" dataDxfId="24" totalsRowDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{C0CE1913-F94A-6640-BCBC-B4DBAA74004F}" name="Proattività" dataDxfId="22">
       <calculatedColumnFormula>Table223452[[#This Row],[Proattività]]</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{EDC08731-1695-884D-81CF-AEADA2B5EB83}" name="Partecipazione"/>
     <tableColumn id="4" xr3:uid="{85E23AA1-A135-344A-B9C5-7B84C9DC1647}" name="Qualità"/>
     <tableColumn id="5" xr3:uid="{F36CD4D3-7F08-3743-99DE-883B443A2608}" name="Relazioni"/>
     <tableColumn id="6" xr3:uid="{2D116FA5-03C4-7B4E-AA2C-5D7DBB07A49D}" name="Rispetto"/>
-    <tableColumn id="10" xr3:uid="{7AA4A5E8-8472-CD45-9E6F-288EB452E431}" name="TOTALE" dataDxfId="44" totalsRowDxfId="23">
+    <tableColumn id="10" xr3:uid="{7AA4A5E8-8472-CD45-9E6F-288EB452E431}" name="TOTALE" dataDxfId="21" totalsRowDxfId="20">
       <calculatedColumnFormula xml:space="preserve"> SUM(B3, C3, D3, E3, F3,) / 5</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -8681,7 +8679,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{39C070D2-A439-4834-B4A1-CDF08BFB0277}" name="Tabella689" displayName="Tabella689" ref="A11:G16" totalsRowShown="0">
   <autoFilter ref="A11:G16" xr:uid="{39C070D2-A439-4834-B4A1-CDF08BFB0277}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{617676FF-0BB4-4C93-842F-A4771B07D6AC}" name="Data" dataDxfId="18" totalsRowDxfId="19"/>
+    <tableColumn id="1" xr3:uid="{617676FF-0BB4-4C93-842F-A4771B07D6AC}" name="Data" dataDxfId="19" totalsRowDxfId="18"/>
     <tableColumn id="2" xr3:uid="{012A2D5D-2F25-479D-9440-C42F880628EC}" name="Proattività" dataDxfId="17">
       <calculatedColumnFormula>Table223452[[#This Row],[Proattività]]</calculatedColumnFormula>
     </tableColumn>
@@ -8689,7 +8687,7 @@
     <tableColumn id="4" xr3:uid="{8557F3DF-FF12-45DB-9C67-3BB8DB9E3F24}" name="Qualità"/>
     <tableColumn id="5" xr3:uid="{4BD330DC-048E-4A9E-B6CD-B5B9FBB6390A}" name="Relazioni"/>
     <tableColumn id="6" xr3:uid="{BA4C168C-A089-4FC6-A040-BAA951A57349}" name="Rispetto"/>
-    <tableColumn id="10" xr3:uid="{8CCDE148-B3B3-42D6-82FE-938326E5E0FD}" name="TOTALE" dataDxfId="15" totalsRowDxfId="16">
+    <tableColumn id="10" xr3:uid="{8CCDE148-B3B3-42D6-82FE-938326E5E0FD}" name="TOTALE" dataDxfId="16" totalsRowDxfId="15">
       <calculatedColumnFormula xml:space="preserve"> SUM(B12, C12, D12, E12, F12,) / 5</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -8701,9 +8699,9 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="9" xr:uid="{F2160B42-3409-45FF-91E3-C1FB03CA8D96}" name="Tabella6810" displayName="Tabella6810" ref="A20:G25" totalsRowShown="0">
   <autoFilter ref="A20:G25" xr:uid="{F2160B42-3409-45FF-91E3-C1FB03CA8D96}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{83366A3D-83CE-4382-B3B0-9D0EB8FE6267}" name="Data" dataDxfId="13" totalsRowDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{ECE9FF42-B3FA-4185-A01B-680319A807F3}" name="Proattività" dataDxfId="12">
-      <calculatedColumnFormula>'18-11-2022'!C5</calculatedColumnFormula>
+    <tableColumn id="1" xr3:uid="{83366A3D-83CE-4382-B3B0-9D0EB8FE6267}" name="Data" dataDxfId="14" totalsRowDxfId="13"/>
+    <tableColumn id="2" xr3:uid="{ECE9FF42-B3FA-4185-A01B-680319A807F3}" name="Proattività" dataDxfId="0">
+      <calculatedColumnFormula>'02-12-2022 '!C4</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{B35E1328-B2B3-4DDE-95D1-5B10B3E78C25}" name="Partecipazione">
       <calculatedColumnFormula>'18-11-2022'!D5</calculatedColumnFormula>
@@ -8717,7 +8715,7 @@
     <tableColumn id="6" xr3:uid="{3173AABA-402D-40FF-86D7-DDADB90ACFE3}" name="Rispetto">
       <calculatedColumnFormula>'18-11-2022'!G5</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{979994A2-EC68-4B40-A526-70C164E26978}" name="TOTALE" dataDxfId="10" totalsRowDxfId="11">
+    <tableColumn id="10" xr3:uid="{979994A2-EC68-4B40-A526-70C164E26978}" name="TOTALE" dataDxfId="12" totalsRowDxfId="11">
       <calculatedColumnFormula xml:space="preserve"> SUM(B21, C21, D21, E21, F21,) / 5</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -8729,10 +8727,8 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{AA98337B-2690-4354-BA56-46929E6E610B}" name="Tabella6811" displayName="Tabella6811" ref="A29:G34" totalsRowShown="0">
   <autoFilter ref="A29:G34" xr:uid="{AA98337B-2690-4354-BA56-46929E6E610B}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{4623CFEB-79C1-464C-ADAB-93C72E3A0683}" name="Data" dataDxfId="8" totalsRowDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{4DC7842C-B300-493B-A908-C480F229B479}" name="Proattività" dataDxfId="7">
-      <calculatedColumnFormula>'18-11-2022'!C6</calculatedColumnFormula>
-    </tableColumn>
+    <tableColumn id="1" xr3:uid="{4623CFEB-79C1-464C-ADAB-93C72E3A0683}" name="Data" dataDxfId="10" totalsRowDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{4DC7842C-B300-493B-A908-C480F229B479}" name="Proattività" dataDxfId="8"/>
     <tableColumn id="3" xr3:uid="{ECFD97D8-A9F8-4ACD-A0AF-9496D7D8138E}" name="Partecipazione">
       <calculatedColumnFormula>'18-11-2022'!D6</calculatedColumnFormula>
     </tableColumn>
@@ -8745,7 +8741,7 @@
     <tableColumn id="6" xr3:uid="{9BEC99AF-9C70-4D75-8DCD-F2A5713A201C}" name="Rispetto">
       <calculatedColumnFormula>'18-11-2022'!G6</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{3D9AADF0-86BA-4499-A5A9-1EACAA5E681B}" name="TOTALE" dataDxfId="5" totalsRowDxfId="6">
+    <tableColumn id="10" xr3:uid="{3D9AADF0-86BA-4499-A5A9-1EACAA5E681B}" name="TOTALE" dataDxfId="7" totalsRowDxfId="6">
       <calculatedColumnFormula xml:space="preserve"> SUM(B30, C30, D30, E30, F30,) / 5</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
@@ -9018,7 +9014,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K59"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
@@ -9105,18 +9101,18 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A7" s="4"/>
-      <c r="B7" s="44"/>
-      <c r="C7" s="44"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="20"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A8" s="4"/>
-      <c r="B8" s="44"/>
-      <c r="C8" s="44"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="20"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.45">
       <c r="A9" s="4"/>
-      <c r="B9" s="44"/>
-      <c r="C9" s="44"/>
+      <c r="B9" s="20"/>
+      <c r="C9" s="20"/>
     </row>
     <row r="11" spans="1:10" ht="43.5" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A11" s="7" t="s">
@@ -9127,14 +9123,14 @@
       <c r="A12" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="25" t="s">
+      <c r="B12" s="48" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="26"/>
-      <c r="G12" s="27"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="49"/>
+      <c r="E12" s="49"/>
+      <c r="F12" s="49"/>
+      <c r="G12" s="50"/>
       <c r="H12" s="10" t="s">
         <v>6</v>
       </c>
@@ -9149,14 +9145,14 @@
       <c r="A13" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B13" s="28" t="s">
+      <c r="B13" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="C13" s="29"/>
-      <c r="D13" s="29"/>
-      <c r="E13" s="29"/>
-      <c r="F13" s="29"/>
-      <c r="G13" s="30"/>
+      <c r="C13" s="34"/>
+      <c r="D13" s="34"/>
+      <c r="E13" s="34"/>
+      <c r="F13" s="34"/>
+      <c r="G13" s="35"/>
       <c r="H13" s="12" t="s">
         <v>11</v>
       </c>
@@ -9171,14 +9167,14 @@
       <c r="A14" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="B14" s="28" t="s">
+      <c r="B14" s="33" t="s">
         <v>48</v>
       </c>
-      <c r="C14" s="29"/>
-      <c r="D14" s="29"/>
-      <c r="E14" s="29"/>
-      <c r="F14" s="29"/>
-      <c r="G14" s="30"/>
+      <c r="C14" s="34"/>
+      <c r="D14" s="34"/>
+      <c r="E14" s="34"/>
+      <c r="F14" s="34"/>
+      <c r="G14" s="35"/>
       <c r="H14" s="15" t="s">
         <v>15</v>
       </c>
@@ -9190,208 +9186,208 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="20.2" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="40" t="s">
+      <c r="A15" s="45" t="s">
         <v>44</v>
       </c>
-      <c r="B15" s="34" t="s">
+      <c r="B15" s="36" t="s">
         <v>18</v>
       </c>
-      <c r="C15" s="35"/>
-      <c r="D15" s="35"/>
-      <c r="E15" s="35"/>
-      <c r="F15" s="35"/>
-      <c r="G15" s="36"/>
-      <c r="H15" s="19" t="s">
+      <c r="C15" s="37"/>
+      <c r="D15" s="37"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="38"/>
+      <c r="H15" s="51" t="s">
         <v>19</v>
       </c>
-      <c r="I15" s="19" t="s">
+      <c r="I15" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="J15" s="19" t="s">
+      <c r="J15" s="51" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="20.2" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="42"/>
-      <c r="B16" s="37" t="s">
+      <c r="A16" s="46"/>
+      <c r="B16" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="39"/>
-      <c r="H16" s="23"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="23"/>
+      <c r="C16" s="40"/>
+      <c r="D16" s="40"/>
+      <c r="E16" s="40"/>
+      <c r="F16" s="40"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="52"/>
+      <c r="J16" s="52"/>
     </row>
     <row r="17" spans="1:11" ht="20.2" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="41"/>
-      <c r="B17" s="31" t="s">
+      <c r="A17" s="47"/>
+      <c r="B17" s="42" t="s">
         <v>41</v>
       </c>
-      <c r="C17" s="32"/>
-      <c r="D17" s="32"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="33"/>
-      <c r="H17" s="20"/>
-      <c r="I17" s="20"/>
-      <c r="J17" s="20"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="44"/>
+      <c r="H17" s="53"/>
+      <c r="I17" s="53"/>
+      <c r="J17" s="53"/>
     </row>
     <row r="18" spans="1:11" ht="20.2" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="40" t="s">
+      <c r="A18" s="45" t="s">
         <v>40</v>
       </c>
-      <c r="B18" s="34" t="s">
+      <c r="B18" s="36" t="s">
         <v>28</v>
       </c>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="19" t="s">
+      <c r="C18" s="37"/>
+      <c r="D18" s="37"/>
+      <c r="E18" s="37"/>
+      <c r="F18" s="37"/>
+      <c r="G18" s="38"/>
+      <c r="H18" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="I18" s="19" t="s">
+      <c r="I18" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="J18" s="21" t="s">
+      <c r="J18" s="54" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="20.2" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="42"/>
-      <c r="B19" s="37" t="s">
+      <c r="A19" s="46"/>
+      <c r="B19" s="39" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="39"/>
-      <c r="H19" s="23"/>
-      <c r="I19" s="23"/>
-      <c r="J19" s="24"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="40"/>
+      <c r="F19" s="40"/>
+      <c r="G19" s="41"/>
+      <c r="H19" s="52"/>
+      <c r="I19" s="52"/>
+      <c r="J19" s="55"/>
     </row>
     <row r="20" spans="1:11" ht="20.2" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="42"/>
-      <c r="B20" s="37" t="s">
+      <c r="A20" s="46"/>
+      <c r="B20" s="39" t="s">
         <v>43</v>
       </c>
-      <c r="C20" s="38"/>
-      <c r="D20" s="38"/>
-      <c r="E20" s="38"/>
-      <c r="F20" s="38"/>
-      <c r="G20" s="39"/>
-      <c r="H20" s="23"/>
-      <c r="I20" s="23"/>
-      <c r="J20" s="24"/>
+      <c r="C20" s="40"/>
+      <c r="D20" s="40"/>
+      <c r="E20" s="40"/>
+      <c r="F20" s="40"/>
+      <c r="G20" s="41"/>
+      <c r="H20" s="52"/>
+      <c r="I20" s="52"/>
+      <c r="J20" s="55"/>
     </row>
     <row r="21" spans="1:11" ht="20.2" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="42"/>
-      <c r="B21" s="37" t="s">
+      <c r="A21" s="46"/>
+      <c r="B21" s="39" t="s">
         <v>26</v>
       </c>
-      <c r="C21" s="38"/>
-      <c r="D21" s="38"/>
-      <c r="E21" s="38"/>
-      <c r="F21" s="38"/>
-      <c r="G21" s="39"/>
-      <c r="H21" s="23"/>
-      <c r="I21" s="23"/>
-      <c r="J21" s="24"/>
+      <c r="C21" s="40"/>
+      <c r="D21" s="40"/>
+      <c r="E21" s="40"/>
+      <c r="F21" s="40"/>
+      <c r="G21" s="41"/>
+      <c r="H21" s="52"/>
+      <c r="I21" s="52"/>
+      <c r="J21" s="55"/>
     </row>
     <row r="22" spans="1:11" ht="20.2" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="41"/>
-      <c r="B22" s="31" t="s">
+      <c r="A22" s="47"/>
+      <c r="B22" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="32"/>
-      <c r="D22" s="32"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="33"/>
-      <c r="H22" s="20"/>
-      <c r="I22" s="20"/>
-      <c r="J22" s="22"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="43"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="44"/>
+      <c r="H22" s="53"/>
+      <c r="I22" s="53"/>
+      <c r="J22" s="56"/>
     </row>
     <row r="23" spans="1:11" ht="20.2" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="40" t="s">
+      <c r="A23" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="B23" s="34" t="s">
+      <c r="B23" s="36" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="35"/>
-      <c r="D23" s="35"/>
-      <c r="E23" s="35"/>
-      <c r="F23" s="35"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="19"/>
-      <c r="I23" s="19"/>
-      <c r="J23" s="21"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="37"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="37"/>
+      <c r="G23" s="38"/>
+      <c r="H23" s="51"/>
+      <c r="I23" s="51"/>
+      <c r="J23" s="54"/>
     </row>
     <row r="24" spans="1:11" ht="18.75" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A24" s="42"/>
-      <c r="B24" s="37" t="s">
+      <c r="A24" s="46"/>
+      <c r="B24" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="38"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="38"/>
-      <c r="G24" s="39"/>
-      <c r="H24" s="23"/>
-      <c r="I24" s="23"/>
-      <c r="J24" s="24"/>
+      <c r="C24" s="40"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="40"/>
+      <c r="F24" s="40"/>
+      <c r="G24" s="41"/>
+      <c r="H24" s="52"/>
+      <c r="I24" s="52"/>
+      <c r="J24" s="55"/>
     </row>
     <row r="25" spans="1:11" ht="18.399999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="42"/>
-      <c r="B25" s="37" t="s">
+      <c r="A25" s="46"/>
+      <c r="B25" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="C25" s="38"/>
-      <c r="D25" s="38"/>
-      <c r="E25" s="38"/>
-      <c r="F25" s="38"/>
-      <c r="G25" s="39"/>
-      <c r="H25" s="23"/>
-      <c r="I25" s="23"/>
-      <c r="J25" s="24"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="40"/>
+      <c r="F25" s="40"/>
+      <c r="G25" s="41"/>
+      <c r="H25" s="52"/>
+      <c r="I25" s="52"/>
+      <c r="J25" s="55"/>
     </row>
     <row r="26" spans="1:11" ht="19.149999999999999" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="41"/>
-      <c r="B26" s="31" t="s">
+      <c r="A26" s="47"/>
+      <c r="B26" s="42" t="s">
         <v>47</v>
       </c>
-      <c r="C26" s="32"/>
-      <c r="D26" s="32"/>
-      <c r="E26" s="32"/>
-      <c r="F26" s="32"/>
-      <c r="G26" s="33"/>
-      <c r="H26" s="20"/>
-      <c r="I26" s="20"/>
-      <c r="J26" s="22"/>
+      <c r="C26" s="43"/>
+      <c r="D26" s="43"/>
+      <c r="E26" s="43"/>
+      <c r="F26" s="43"/>
+      <c r="G26" s="44"/>
+      <c r="H26" s="53"/>
+      <c r="I26" s="53"/>
+      <c r="J26" s="56"/>
     </row>
     <row r="27" spans="1:11" ht="25.05" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A27" s="4"/>
-      <c r="B27" s="43"/>
-      <c r="C27" s="43"/>
-      <c r="D27" s="43"/>
-      <c r="E27" s="43"/>
-      <c r="F27" s="43"/>
-      <c r="G27" s="43"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="19"/>
+      <c r="D27" s="19"/>
+      <c r="E27" s="19"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
       <c r="J27" s="1"/>
     </row>
     <row r="28" spans="1:11" ht="29.55" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B28" s="43"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="43"/>
+      <c r="B28" s="19"/>
+      <c r="C28" s="19"/>
+      <c r="D28" s="19"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="19"/>
       <c r="J28" s="1"/>
     </row>
     <row r="29" spans="1:11" ht="31.05" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -9544,16 +9540,15 @@
     <protectedRange password="E169" sqref="A2:C9 A18:A28 A50:A57 A31:A42" name="Intervallo1"/>
   </protectedRanges>
   <mergeCells count="27">
-    <mergeCell ref="B13:G13"/>
-    <mergeCell ref="B14:G14"/>
-    <mergeCell ref="B15:G15"/>
-    <mergeCell ref="B16:G16"/>
-    <mergeCell ref="B17:G17"/>
-    <mergeCell ref="A15:A17"/>
-    <mergeCell ref="A18:A22"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="B20:G20"/>
-    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="H23:H26"/>
+    <mergeCell ref="I23:I26"/>
+    <mergeCell ref="J23:J26"/>
+    <mergeCell ref="H15:H17"/>
+    <mergeCell ref="I15:I17"/>
+    <mergeCell ref="J15:J17"/>
+    <mergeCell ref="H18:H22"/>
+    <mergeCell ref="I18:I22"/>
+    <mergeCell ref="J18:J22"/>
     <mergeCell ref="B24:G24"/>
     <mergeCell ref="A23:A26"/>
     <mergeCell ref="B12:G12"/>
@@ -9562,15 +9557,16 @@
     <mergeCell ref="B22:G22"/>
     <mergeCell ref="B19:G19"/>
     <mergeCell ref="B25:G25"/>
-    <mergeCell ref="H15:H17"/>
-    <mergeCell ref="I15:I17"/>
-    <mergeCell ref="J15:J17"/>
-    <mergeCell ref="H18:H22"/>
-    <mergeCell ref="I18:I22"/>
-    <mergeCell ref="J18:J22"/>
-    <mergeCell ref="H23:H26"/>
-    <mergeCell ref="I23:I26"/>
-    <mergeCell ref="J23:J26"/>
+    <mergeCell ref="A15:A17"/>
+    <mergeCell ref="A18:A22"/>
+    <mergeCell ref="B18:G18"/>
+    <mergeCell ref="B20:G20"/>
+    <mergeCell ref="B21:G21"/>
+    <mergeCell ref="B13:G13"/>
+    <mergeCell ref="B14:G14"/>
+    <mergeCell ref="B15:G15"/>
+    <mergeCell ref="B16:G16"/>
+    <mergeCell ref="B17:G17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -9582,7 +9578,7 @@
   <dimension ref="A1:K10"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -9643,11 +9639,28 @@
         <f>CONCATENATE(Legenda!B2," ",Legenda!C2)</f>
         <v>Alessandro Borrelli</v>
       </c>
+      <c r="C3">
+        <v>8</v>
+      </c>
+      <c r="D3">
+        <v>7</v>
+      </c>
+      <c r="E3">
+        <v>9</v>
+      </c>
+      <c r="F3">
+        <v>10</v>
+      </c>
+      <c r="G3">
+        <v>10</v>
+      </c>
       <c r="H3" s="1">
         <f xml:space="preserve"> SUM(C3,D3,E3,F3,G3)/5</f>
-        <v>0</v>
-      </c>
-      <c r="I3" s="5"/>
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="I3" s="5">
+        <v>9</v>
+      </c>
     </row>
     <row r="4" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A4" s="6">
@@ -9658,11 +9671,28 @@
         <f>CONCATENATE(Legenda!B3," ",Legenda!C3)</f>
         <v>Vincenzo Cerciello</v>
       </c>
+      <c r="C4">
+        <v>9</v>
+      </c>
+      <c r="D4">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>8</v>
+      </c>
+      <c r="F4">
+        <v>10</v>
+      </c>
+      <c r="G4">
+        <v>10</v>
+      </c>
       <c r="H4" s="1">
         <f xml:space="preserve"> SUM(C4,D4,E4,F4,G4)/5</f>
-        <v>0</v>
-      </c>
-      <c r="I4" s="5"/>
+        <v>9.4</v>
+      </c>
+      <c r="I4" s="5">
+        <v>9.5</v>
+      </c>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A5" s="6">
@@ -9673,11 +9703,28 @@
         <f>CONCATENATE(Legenda!B4," ",Legenda!C4)</f>
         <v>Michela Faella</v>
       </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>10</v>
+      </c>
+      <c r="E5">
+        <v>9</v>
+      </c>
+      <c r="F5">
+        <v>10</v>
+      </c>
+      <c r="G5">
+        <v>10</v>
+      </c>
       <c r="H5" s="1">
         <f xml:space="preserve"> SUM(C5,D5,E5,F5,G5)/5</f>
-        <v>0</v>
-      </c>
-      <c r="I5" s="5"/>
+        <v>9.8000000000000007</v>
+      </c>
+      <c r="I5" s="5">
+        <v>10</v>
+      </c>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A6" s="6">
@@ -9688,11 +9735,28 @@
         <f>CONCATENATE(Legenda!B5," ",Legenda!C5)</f>
         <v>Gerardo Francesco Napolitano</v>
       </c>
+      <c r="C6">
+        <v>9</v>
+      </c>
+      <c r="D6">
+        <v>10</v>
+      </c>
+      <c r="E6">
+        <v>9</v>
+      </c>
+      <c r="F6">
+        <v>10</v>
+      </c>
+      <c r="G6">
+        <v>10</v>
+      </c>
       <c r="H6" s="1">
         <f xml:space="preserve"> SUM(C6,D6,E6,F6,G6)/5</f>
-        <v>0</v>
-      </c>
-      <c r="I6" s="5"/>
+        <v>9.6</v>
+      </c>
+      <c r="I6" s="5">
+        <v>9.5</v>
+      </c>
     </row>
     <row r="7" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A7" s="6">
@@ -9703,11 +9767,28 @@
         <f>CONCATENATE(Legenda!B6," ",Legenda!C6)</f>
         <v>Mirko Vitale</v>
       </c>
+      <c r="C7">
+        <v>9</v>
+      </c>
+      <c r="D7">
+        <v>10</v>
+      </c>
+      <c r="E7">
+        <v>9</v>
+      </c>
+      <c r="F7">
+        <v>10</v>
+      </c>
+      <c r="G7">
+        <v>10</v>
+      </c>
       <c r="H7" s="1">
         <f>SUM(C7,D7,E7,F7,G7)/5</f>
-        <v>0</v>
-      </c>
-      <c r="I7" s="5"/>
+        <v>9.6</v>
+      </c>
+      <c r="I7" s="5">
+        <v>9.5</v>
+      </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A8" s="6"/>
@@ -10388,7 +10469,7 @@
   <dimension ref="A1:P77"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J44" sqref="J44"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -10445,27 +10526,27 @@
       </c>
       <c r="B3">
         <f>Table223452[[#This Row],[Proattività]]</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C3">
         <f>Table223452[[#This Row],[Partecipazione]]</f>
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="D3">
         <f>Table223452[[#This Row],[Qualità]]</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E3">
         <f>Table223452[[#This Row],[Relazioni]]</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F3">
         <f>Table223452[[#This Row],[Rispetto]]</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G3" s="1">
         <f xml:space="preserve"> SUM(B3, C3, D3, E3, F3,) / 5</f>
-        <v>0</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="I3" s="18"/>
       <c r="K3"/>
@@ -10599,8 +10680,8 @@
         <f>CONCATENATE(Legenda!B3," ",Legenda!C3)</f>
         <v>Vincenzo Cerciello</v>
       </c>
-      <c r="J10" s="45"/>
-      <c r="K10" s="46"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="22"/>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A11" s="14" t="s">
@@ -10627,8 +10708,8 @@
       <c r="I11" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="J11" s="45"/>
-      <c r="K11" s="48"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="24"/>
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A12" s="14">
@@ -10636,31 +10717,31 @@
       </c>
       <c r="B12">
         <f>'18-11-2022'!C4</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C12">
         <f>'18-11-2022'!D4</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D12">
         <f>'18-11-2022'!E4</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="E12">
         <f>'18-11-2022'!F4</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F12">
         <f>'18-11-2022'!G4</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G12" s="1">
         <f xml:space="preserve"> SUM(B12, C12, D12, E12, F12,) / 5</f>
-        <v>0</v>
+        <v>9.4</v>
       </c>
       <c r="I12" s="18"/>
-      <c r="J12" s="45"/>
-      <c r="K12" s="46"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="22"/>
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A13" s="14">
@@ -10691,8 +10772,8 @@
         <v>0</v>
       </c>
       <c r="I13" s="5"/>
-      <c r="J13" s="45"/>
-      <c r="K13" s="46"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="22"/>
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A14" s="14">
@@ -10723,8 +10804,8 @@
         <v>0</v>
       </c>
       <c r="I14" s="5"/>
-      <c r="J14" s="45"/>
-      <c r="K14" s="46"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="22"/>
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A15" s="14">
@@ -10755,8 +10836,8 @@
         <v>0</v>
       </c>
       <c r="I15" s="5"/>
-      <c r="J15" s="45"/>
-      <c r="K15" s="46"/>
+      <c r="J15" s="21"/>
+      <c r="K15" s="22"/>
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A16" s="14">
@@ -10787,42 +10868,42 @@
         <v>0</v>
       </c>
       <c r="I16" s="5"/>
-      <c r="J16" s="45"/>
-      <c r="K16" s="46"/>
+      <c r="J16" s="21"/>
+      <c r="K16" s="22"/>
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A17" s="47"/>
-      <c r="B17" s="45"/>
-      <c r="C17" s="45"/>
-      <c r="D17" s="45"/>
-      <c r="E17" s="45"/>
-      <c r="F17" s="45"/>
-      <c r="G17" s="45"/>
-      <c r="H17" s="45"/>
-      <c r="I17" s="49"/>
-      <c r="J17" s="45"/>
-      <c r="K17" s="46"/>
+      <c r="A17" s="23"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="25"/>
+      <c r="J17" s="21"/>
+      <c r="K17" s="22"/>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A18" s="47"/>
-      <c r="B18" s="45"/>
-      <c r="C18" s="45"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="45"/>
-      <c r="F18" s="45"/>
-      <c r="G18" s="45"/>
-      <c r="H18" s="45"/>
-      <c r="I18" s="45"/>
-      <c r="J18" s="45"/>
-      <c r="K18" s="46"/>
+      <c r="A18" s="23"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="22"/>
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A19" s="14" t="str">
         <f>CONCATENATE(Legenda!B4," ",Legenda!C4)</f>
         <v>Michela Faella</v>
       </c>
-      <c r="J19" s="45"/>
-      <c r="K19" s="46"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="22"/>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A20" s="14" t="s">
@@ -10849,8 +10930,8 @@
       <c r="I20" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="J20" s="45"/>
-      <c r="K20" s="46"/>
+      <c r="J20" s="21"/>
+      <c r="K20" s="22"/>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A21" s="14">
@@ -10858,54 +10939,54 @@
       </c>
       <c r="B21">
         <f>'18-11-2022'!C5</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C21">
         <f>'18-11-2022'!D5</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D21">
         <f>'18-11-2022'!E5</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E21">
         <f>'18-11-2022'!F5</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F21">
         <f>'18-11-2022'!G5</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G21" s="1">
         <f xml:space="preserve"> SUM(B21, C21, D21, E21, F21,) / 5</f>
-        <v>0</v>
+        <v>9.8000000000000007</v>
       </c>
       <c r="I21" s="18"/>
-      <c r="J21" s="45"/>
-      <c r="K21" s="48"/>
+      <c r="J21" s="21"/>
+      <c r="K21" s="24"/>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A22" s="14">
         <v>44897</v>
       </c>
       <c r="B22">
-        <f>'18-11-2022'!C6</f>
+        <f>'02-12-2022 '!C5</f>
         <v>0</v>
       </c>
       <c r="C22">
-        <f>'18-11-2022'!D6</f>
+        <f>'02-12-2022 '!D5</f>
         <v>0</v>
       </c>
       <c r="D22">
-        <f>'18-11-2022'!E6</f>
+        <f>'02-12-2022 '!E5</f>
         <v>0</v>
       </c>
       <c r="E22">
-        <f>'18-11-2022'!F6</f>
+        <f>'02-12-2022 '!F5</f>
         <v>0</v>
       </c>
       <c r="F22">
-        <f>'18-11-2022'!G6</f>
+        <f>'02-12-2022 '!G5</f>
         <v>0</v>
       </c>
       <c r="G22" s="1">
@@ -10913,31 +10994,31 @@
         <v>0</v>
       </c>
       <c r="I22" s="5"/>
-      <c r="J22" s="45"/>
-      <c r="K22" s="46"/>
+      <c r="J22" s="21"/>
+      <c r="K22" s="22"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A23" s="14">
         <v>44911</v>
       </c>
       <c r="B23">
-        <f>'18-11-2022'!C7</f>
+        <f>'16-12-2022 '!C5</f>
         <v>0</v>
       </c>
       <c r="C23">
-        <f>'18-11-2022'!D7</f>
+        <f>'16-12-2022 '!D5</f>
         <v>0</v>
       </c>
       <c r="D23">
-        <f>'18-11-2022'!E7</f>
+        <f>'16-12-2022 '!E5</f>
         <v>0</v>
       </c>
       <c r="E23">
-        <f>'18-11-2022'!F7</f>
+        <f>'16-12-2022 '!F5</f>
         <v>0</v>
       </c>
       <c r="F23">
-        <f>'18-11-2022'!G7</f>
+        <f>'16-12-2022 '!G5</f>
         <v>0</v>
       </c>
       <c r="G23" s="1">
@@ -10945,31 +11026,31 @@
         <v>0</v>
       </c>
       <c r="I23" s="5"/>
-      <c r="J23" s="45"/>
-      <c r="K23" s="46"/>
+      <c r="J23" s="21"/>
+      <c r="K23" s="22"/>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A24" s="14">
         <v>44925</v>
       </c>
       <c r="B24">
-        <f>'18-11-2022'!C8</f>
+        <f>'30-12-2022 '!C5</f>
         <v>0</v>
       </c>
       <c r="C24">
-        <f>'18-11-2022'!D8</f>
+        <f>'30-12-2022 '!D5</f>
         <v>0</v>
       </c>
       <c r="D24">
-        <f>'18-11-2022'!E8</f>
+        <f>'30-12-2022 '!E5</f>
         <v>0</v>
       </c>
       <c r="E24">
-        <f>'18-11-2022'!F8</f>
+        <f>'30-12-2022 '!F5</f>
         <v>0</v>
       </c>
       <c r="F24">
-        <f>'18-11-2022'!G8</f>
+        <f>'30-12-2022 '!G5</f>
         <v>0</v>
       </c>
       <c r="G24" s="1">
@@ -10977,31 +11058,31 @@
         <v>0</v>
       </c>
       <c r="I24" s="5"/>
-      <c r="J24" s="45"/>
-      <c r="K24" s="46"/>
+      <c r="J24" s="21"/>
+      <c r="K24" s="22"/>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A25" s="14">
         <v>44939</v>
       </c>
       <c r="B25">
-        <f>'18-11-2022'!C9</f>
+        <f>'13-01-2023 '!C5</f>
         <v>0</v>
       </c>
       <c r="C25">
-        <f>'18-11-2022'!D9</f>
+        <f>'13-01-2023 '!D5</f>
         <v>0</v>
       </c>
       <c r="D25">
-        <f>'18-11-2022'!E9</f>
+        <f>'13-01-2023 '!E5</f>
         <v>0</v>
       </c>
       <c r="E25">
-        <f>'18-11-2022'!F9</f>
+        <f>'13-01-2023 '!F5</f>
         <v>0</v>
       </c>
       <c r="F25">
-        <f>'18-11-2022'!G9</f>
+        <f>'13-01-2023 '!G5</f>
         <v>0</v>
       </c>
       <c r="G25" s="1">
@@ -11009,42 +11090,42 @@
         <v>0</v>
       </c>
       <c r="I25" s="5"/>
-      <c r="J25" s="45"/>
-      <c r="K25" s="46"/>
+      <c r="J25" s="21"/>
+      <c r="K25" s="22"/>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A26" s="47"/>
-      <c r="B26" s="45"/>
-      <c r="C26" s="45"/>
-      <c r="D26" s="45"/>
-      <c r="E26" s="45"/>
-      <c r="F26" s="45"/>
-      <c r="G26" s="45"/>
-      <c r="H26" s="45"/>
-      <c r="I26" s="49"/>
-      <c r="J26" s="45"/>
-      <c r="K26" s="46"/>
+      <c r="A26" s="23"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="25"/>
+      <c r="J26" s="21"/>
+      <c r="K26" s="22"/>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A27" s="47"/>
-      <c r="B27" s="45"/>
-      <c r="C27" s="45"/>
-      <c r="D27" s="45"/>
-      <c r="E27" s="45"/>
-      <c r="F27" s="45"/>
-      <c r="G27" s="45"/>
-      <c r="H27" s="45"/>
-      <c r="I27" s="49"/>
-      <c r="J27" s="45"/>
-      <c r="K27" s="46"/>
+      <c r="A27" s="23"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="25"/>
+      <c r="J27" s="21"/>
+      <c r="K27" s="22"/>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A28" s="14" t="str">
         <f>CONCATENATE(Legenda!B5," ",Legenda!C5)</f>
         <v>Gerardo Francesco Napolitano</v>
       </c>
-      <c r="J28" s="45"/>
-      <c r="K28" s="46"/>
+      <c r="J28" s="21"/>
+      <c r="K28" s="22"/>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A29" s="14" t="s">
@@ -11071,8 +11152,8 @@
       <c r="I29" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="J29" s="45"/>
-      <c r="K29" s="46"/>
+      <c r="J29" s="21"/>
+      <c r="K29" s="22"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A30" s="14">
@@ -11080,54 +11161,54 @@
       </c>
       <c r="B30">
         <f>'18-11-2022'!C6</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C30">
         <f>'18-11-2022'!D6</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D30">
         <f>'18-11-2022'!E6</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E30">
         <f>'18-11-2022'!F6</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F30">
         <f>'18-11-2022'!G6</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G30" s="1">
         <f xml:space="preserve"> SUM(B30, C30, D30, E30, F30,) / 5</f>
-        <v>0</v>
+        <v>9.6</v>
       </c>
       <c r="I30" s="18"/>
-      <c r="J30" s="45"/>
-      <c r="K30" s="46"/>
+      <c r="J30" s="21"/>
+      <c r="K30" s="22"/>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A31" s="14">
         <v>44897</v>
       </c>
       <c r="B31">
-        <f>'18-11-2022'!C7</f>
+        <f>'02-12-2022 '!C6</f>
         <v>0</v>
       </c>
       <c r="C31">
-        <f>'18-11-2022'!D7</f>
+        <f>'02-12-2022 '!D6</f>
         <v>0</v>
       </c>
       <c r="D31">
-        <f>'18-11-2022'!E7</f>
+        <f>'02-12-2022 '!E6</f>
         <v>0</v>
       </c>
       <c r="E31">
-        <f>'18-11-2022'!F7</f>
+        <f>'02-12-2022 '!F6</f>
         <v>0</v>
       </c>
       <c r="F31">
-        <f>'18-11-2022'!G7</f>
+        <f>'02-12-2022 '!G6</f>
         <v>0</v>
       </c>
       <c r="G31" s="1">
@@ -11135,31 +11216,31 @@
         <v>0</v>
       </c>
       <c r="I31" s="5"/>
-      <c r="J31" s="45"/>
-      <c r="K31" s="48"/>
+      <c r="J31" s="21"/>
+      <c r="K31" s="24"/>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A32" s="14">
         <v>44911</v>
       </c>
       <c r="B32">
-        <f>'18-11-2022'!C8</f>
+        <f>'16-12-2022 '!C6</f>
         <v>0</v>
       </c>
       <c r="C32">
-        <f>'18-11-2022'!D8</f>
+        <f>'16-12-2022 '!D6</f>
         <v>0</v>
       </c>
       <c r="D32">
-        <f>'18-11-2022'!E8</f>
+        <f>'16-12-2022 '!E6</f>
         <v>0</v>
       </c>
       <c r="E32">
-        <f>'18-11-2022'!F8</f>
+        <f>'16-12-2022 '!F6</f>
         <v>0</v>
       </c>
       <c r="F32">
-        <f>'18-11-2022'!G8</f>
+        <f>'16-12-2022 '!G6</f>
         <v>0</v>
       </c>
       <c r="G32" s="1">
@@ -11167,63 +11248,63 @@
         <v>0</v>
       </c>
       <c r="I32" s="5"/>
-      <c r="J32" s="45"/>
-      <c r="K32" s="46"/>
+      <c r="J32" s="21"/>
+      <c r="K32" s="22"/>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A33" s="14">
         <v>44925</v>
       </c>
       <c r="B33">
-        <f>'18-11-2022'!C9</f>
+        <f>'30-12-2022 '!C6</f>
         <v>0</v>
       </c>
       <c r="C33">
-        <f>'18-11-2022'!D9</f>
+        <f>'30-12-2022 '!D6</f>
         <v>0</v>
       </c>
       <c r="D33">
-        <f>'18-11-2022'!E9</f>
+        <f>'30-12-2022 '!E6</f>
         <v>0</v>
       </c>
       <c r="E33">
-        <f>'18-11-2022'!F9</f>
+        <f>'30-12-2022 '!F6</f>
         <v>0</v>
       </c>
       <c r="F33">
-        <f>'18-11-2022'!G9</f>
+        <f>'30-12-2022 '!G6</f>
         <v>0</v>
       </c>
       <c r="G33" s="1">
-        <f t="shared" si="3"/>
+        <f xml:space="preserve"> SUM(B33, C33, D33, E33, F33,) / 5</f>
         <v>0</v>
       </c>
       <c r="I33" s="5"/>
-      <c r="J33" s="45"/>
-      <c r="K33" s="46"/>
+      <c r="J33" s="21"/>
+      <c r="K33" s="22"/>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A34" s="14">
         <v>44939</v>
       </c>
       <c r="B34">
-        <f>'18-11-2022'!C10</f>
+        <f>'13-01-2023 '!C6</f>
         <v>0</v>
       </c>
       <c r="C34">
-        <f>'18-11-2022'!D10</f>
+        <f>'13-01-2023 '!D6</f>
         <v>0</v>
       </c>
       <c r="D34">
-        <f>'18-11-2022'!E10</f>
+        <f>'13-01-2023 '!E6</f>
         <v>0</v>
       </c>
       <c r="E34">
-        <f>'18-11-2022'!F10</f>
+        <f>'13-01-2023 '!F6</f>
         <v>0</v>
       </c>
       <c r="F34">
-        <f>'18-11-2022'!G10</f>
+        <f>'13-01-2023 '!G6</f>
         <v>0</v>
       </c>
       <c r="G34" s="1">
@@ -11231,42 +11312,42 @@
         <v>0</v>
       </c>
       <c r="I34" s="5"/>
-      <c r="J34" s="45"/>
-      <c r="K34" s="46"/>
+      <c r="J34" s="21"/>
+      <c r="K34" s="22"/>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A35" s="50"/>
-      <c r="B35" s="54"/>
-      <c r="C35" s="54"/>
-      <c r="D35" s="54"/>
-      <c r="E35" s="54"/>
-      <c r="F35" s="54"/>
-      <c r="G35" s="54"/>
-      <c r="H35" s="54"/>
-      <c r="I35" s="55"/>
-      <c r="J35" s="45"/>
-      <c r="K35" s="46"/>
+      <c r="A35" s="26"/>
+      <c r="B35" s="30"/>
+      <c r="C35" s="30"/>
+      <c r="D35" s="30"/>
+      <c r="E35" s="30"/>
+      <c r="F35" s="30"/>
+      <c r="G35" s="30"/>
+      <c r="H35" s="30"/>
+      <c r="I35" s="31"/>
+      <c r="J35" s="21"/>
+      <c r="K35" s="22"/>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A36" s="50"/>
-      <c r="B36" s="54"/>
-      <c r="C36" s="54"/>
-      <c r="D36" s="54"/>
-      <c r="E36" s="54"/>
-      <c r="F36" s="54"/>
-      <c r="G36" s="54"/>
-      <c r="H36" s="54"/>
-      <c r="I36" s="55"/>
-      <c r="J36" s="45"/>
-      <c r="K36" s="46"/>
+      <c r="A36" s="26"/>
+      <c r="B36" s="30"/>
+      <c r="C36" s="30"/>
+      <c r="D36" s="30"/>
+      <c r="E36" s="30"/>
+      <c r="F36" s="30"/>
+      <c r="G36" s="30"/>
+      <c r="H36" s="30"/>
+      <c r="I36" s="31"/>
+      <c r="J36" s="21"/>
+      <c r="K36" s="22"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A37" s="14" t="str">
         <f>CONCATENATE(Legenda!B6," ",Legenda!C6)</f>
         <v>Mirko Vitale</v>
       </c>
-      <c r="J37" s="45"/>
-      <c r="K37" s="46"/>
+      <c r="J37" s="21"/>
+      <c r="K37" s="22"/>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A38" s="14" t="s">
@@ -11293,8 +11374,8 @@
       <c r="I38" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="J38" s="45"/>
-      <c r="K38" s="46"/>
+      <c r="J38" s="21"/>
+      <c r="K38" s="22"/>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A39" s="14">
@@ -11302,54 +11383,54 @@
       </c>
       <c r="B39">
         <f>'18-11-2022'!C7</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="C39">
         <f>'18-11-2022'!D7</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D39">
         <f>'18-11-2022'!E7</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="E39">
         <f>'18-11-2022'!F7</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="F39">
         <f>'18-11-2022'!G7</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="G39" s="1">
         <f xml:space="preserve"> SUM(B39, C39, D39, E39, F39,) / 5</f>
-        <v>0</v>
+        <v>9.6</v>
       </c>
       <c r="I39" s="18"/>
-      <c r="J39" s="45"/>
-      <c r="K39" s="46"/>
+      <c r="J39" s="21"/>
+      <c r="K39" s="22"/>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A40" s="14">
         <v>44897</v>
       </c>
       <c r="B40">
-        <f>'18-11-2022'!C8</f>
+        <f>'02-12-2022 '!C7</f>
         <v>0</v>
       </c>
       <c r="C40">
-        <f>'18-11-2022'!D8</f>
+        <f>'02-12-2022 '!D7</f>
         <v>0</v>
       </c>
       <c r="D40">
-        <f>'18-11-2022'!E8</f>
+        <f>'02-12-2022 '!E7</f>
         <v>0</v>
       </c>
       <c r="E40">
-        <f>'18-11-2022'!F8</f>
+        <f>'02-12-2022 '!F7</f>
         <v>0</v>
       </c>
       <c r="F40">
-        <f>'18-11-2022'!G8</f>
+        <f>'02-12-2022 '!G7</f>
         <v>0</v>
       </c>
       <c r="G40" s="1">
@@ -11357,31 +11438,31 @@
         <v>0</v>
       </c>
       <c r="I40" s="5"/>
-      <c r="J40" s="45"/>
-      <c r="K40" s="46"/>
+      <c r="J40" s="21"/>
+      <c r="K40" s="22"/>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A41" s="14">
         <v>44911</v>
       </c>
       <c r="B41">
-        <f>'18-11-2022'!C9</f>
+        <f>'16-12-2022 '!C7</f>
         <v>0</v>
       </c>
       <c r="C41">
-        <f>'18-11-2022'!D9</f>
+        <f>'16-12-2022 '!D7</f>
         <v>0</v>
       </c>
       <c r="D41">
-        <f>'18-11-2022'!E9</f>
+        <f>'16-12-2022 '!E7</f>
         <v>0</v>
       </c>
       <c r="E41">
-        <f>'18-11-2022'!F9</f>
+        <f>'16-12-2022 '!F7</f>
         <v>0</v>
       </c>
       <c r="F41">
-        <f>'18-11-2022'!G9</f>
+        <f>'16-12-2022 '!G7</f>
         <v>0</v>
       </c>
       <c r="G41" s="1">
@@ -11389,31 +11470,31 @@
         <v>0</v>
       </c>
       <c r="I41" s="5"/>
-      <c r="J41" s="45"/>
-      <c r="K41" s="48"/>
+      <c r="J41" s="21"/>
+      <c r="K41" s="24"/>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A42" s="14">
         <v>44925</v>
       </c>
       <c r="B42">
-        <f>'18-11-2022'!C10</f>
+        <f>'30-12-2022 '!C7</f>
         <v>0</v>
       </c>
       <c r="C42">
-        <f>'18-11-2022'!D10</f>
+        <f>'30-12-2022 '!D7</f>
         <v>0</v>
       </c>
       <c r="D42">
-        <f>'18-11-2022'!E10</f>
+        <f>'30-12-2022 '!E7</f>
         <v>0</v>
       </c>
       <c r="E42">
-        <f>'18-11-2022'!F10</f>
+        <f>'30-12-2022 '!F7</f>
         <v>0</v>
       </c>
       <c r="F42">
-        <f>'18-11-2022'!G10</f>
+        <f>'30-12-2022 '!G7</f>
         <v>0</v>
       </c>
       <c r="G42" s="1">
@@ -11421,31 +11502,31 @@
         <v>0</v>
       </c>
       <c r="I42" s="5"/>
-      <c r="J42" s="45"/>
-      <c r="K42" s="46"/>
+      <c r="J42" s="21"/>
+      <c r="K42" s="22"/>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.45">
       <c r="A43" s="14">
         <v>44939</v>
       </c>
       <c r="B43">
-        <f>'18-11-2022'!C11</f>
+        <f>'13-01-2023 '!C7</f>
         <v>0</v>
       </c>
       <c r="C43">
-        <f>'18-11-2022'!D11</f>
+        <f>'13-01-2023 '!D7</f>
         <v>0</v>
       </c>
       <c r="D43">
-        <f>'18-11-2022'!E11</f>
+        <f>'13-01-2023 '!E7</f>
         <v>0</v>
       </c>
       <c r="E43">
-        <f>'18-11-2022'!F11</f>
+        <f>'13-01-2023 '!F7</f>
         <v>0</v>
       </c>
       <c r="F43">
-        <f>'18-11-2022'!G11</f>
+        <f>'13-01-2023 '!G7</f>
         <v>0</v>
       </c>
       <c r="G43" s="1">
@@ -11453,450 +11534,450 @@
         <v>0</v>
       </c>
       <c r="I43" s="5"/>
-      <c r="J43" s="45"/>
-      <c r="K43" s="46"/>
+      <c r="J43" s="21"/>
+      <c r="K43" s="22"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A44" s="50"/>
-      <c r="B44" s="54"/>
-      <c r="C44" s="54"/>
-      <c r="D44" s="54"/>
-      <c r="E44" s="54"/>
-      <c r="F44" s="54"/>
-      <c r="G44" s="54"/>
-      <c r="H44" s="54"/>
-      <c r="I44" s="55"/>
-      <c r="J44" s="45"/>
-      <c r="K44" s="46"/>
+      <c r="A44" s="26"/>
+      <c r="B44" s="30"/>
+      <c r="C44" s="30"/>
+      <c r="D44" s="30"/>
+      <c r="E44" s="30"/>
+      <c r="F44" s="30"/>
+      <c r="G44" s="30"/>
+      <c r="H44" s="30"/>
+      <c r="I44" s="31"/>
+      <c r="J44" s="21"/>
+      <c r="K44" s="22"/>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A45" s="50"/>
-      <c r="B45" s="54"/>
-      <c r="C45" s="54"/>
-      <c r="D45" s="54"/>
-      <c r="E45" s="54"/>
-      <c r="F45" s="54"/>
-      <c r="G45" s="54"/>
-      <c r="H45" s="54"/>
-      <c r="I45" s="55"/>
-      <c r="J45" s="45"/>
-      <c r="K45" s="46"/>
+      <c r="A45" s="26"/>
+      <c r="B45" s="30"/>
+      <c r="C45" s="30"/>
+      <c r="D45" s="30"/>
+      <c r="E45" s="30"/>
+      <c r="F45" s="30"/>
+      <c r="G45" s="30"/>
+      <c r="H45" s="30"/>
+      <c r="I45" s="31"/>
+      <c r="J45" s="21"/>
+      <c r="K45" s="22"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A46" s="50"/>
-      <c r="B46" s="54"/>
-      <c r="C46" s="54"/>
-      <c r="D46" s="54"/>
-      <c r="E46" s="54"/>
-      <c r="F46" s="54"/>
-      <c r="G46" s="54"/>
-      <c r="H46" s="54"/>
-      <c r="I46" s="55"/>
-      <c r="J46" s="45"/>
-      <c r="K46" s="46"/>
+      <c r="A46" s="26"/>
+      <c r="B46" s="30"/>
+      <c r="C46" s="30"/>
+      <c r="D46" s="30"/>
+      <c r="E46" s="30"/>
+      <c r="F46" s="30"/>
+      <c r="G46" s="30"/>
+      <c r="H46" s="30"/>
+      <c r="I46" s="31"/>
+      <c r="J46" s="21"/>
+      <c r="K46" s="22"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A47" s="47"/>
-      <c r="B47" s="45"/>
-      <c r="C47" s="45"/>
-      <c r="D47" s="45"/>
-      <c r="E47" s="45"/>
-      <c r="F47" s="45"/>
-      <c r="G47" s="45"/>
-      <c r="H47" s="45"/>
-      <c r="I47" s="56"/>
-      <c r="J47" s="45"/>
-      <c r="K47" s="46"/>
+      <c r="A47" s="23"/>
+      <c r="B47" s="21"/>
+      <c r="C47" s="21"/>
+      <c r="D47" s="21"/>
+      <c r="E47" s="21"/>
+      <c r="F47" s="21"/>
+      <c r="G47" s="21"/>
+      <c r="H47" s="21"/>
+      <c r="I47" s="32"/>
+      <c r="J47" s="21"/>
+      <c r="K47" s="22"/>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A48" s="47"/>
-      <c r="B48" s="45"/>
-      <c r="C48" s="45"/>
-      <c r="D48" s="45"/>
-      <c r="E48" s="45"/>
-      <c r="F48" s="45"/>
-      <c r="G48" s="45"/>
-      <c r="H48" s="45"/>
-      <c r="I48" s="45"/>
-      <c r="J48" s="45"/>
-      <c r="K48" s="46"/>
+      <c r="A48" s="23"/>
+      <c r="B48" s="21"/>
+      <c r="C48" s="21"/>
+      <c r="D48" s="21"/>
+      <c r="E48" s="21"/>
+      <c r="F48" s="21"/>
+      <c r="G48" s="21"/>
+      <c r="H48" s="21"/>
+      <c r="I48" s="21"/>
+      <c r="J48" s="21"/>
+      <c r="K48" s="22"/>
     </row>
     <row r="49" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A49" s="47"/>
-      <c r="B49" s="45"/>
-      <c r="C49" s="45"/>
-      <c r="D49" s="45"/>
-      <c r="E49" s="45"/>
-      <c r="F49" s="45"/>
-      <c r="G49" s="45"/>
-      <c r="H49" s="45"/>
-      <c r="I49" s="45"/>
-      <c r="J49" s="45"/>
-      <c r="K49" s="46"/>
+      <c r="A49" s="23"/>
+      <c r="B49" s="21"/>
+      <c r="C49" s="21"/>
+      <c r="D49" s="21"/>
+      <c r="E49" s="21"/>
+      <c r="F49" s="21"/>
+      <c r="G49" s="21"/>
+      <c r="H49" s="21"/>
+      <c r="I49" s="21"/>
+      <c r="J49" s="21"/>
+      <c r="K49" s="22"/>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A50" s="50"/>
-      <c r="B50" s="51"/>
-      <c r="C50" s="51"/>
-      <c r="D50" s="51"/>
-      <c r="E50" s="51"/>
-      <c r="F50" s="51"/>
-      <c r="G50" s="51"/>
-      <c r="H50" s="51"/>
-      <c r="I50" s="51"/>
-      <c r="J50" s="45"/>
-      <c r="K50" s="46"/>
+      <c r="A50" s="26"/>
+      <c r="B50" s="27"/>
+      <c r="C50" s="27"/>
+      <c r="D50" s="27"/>
+      <c r="E50" s="27"/>
+      <c r="F50" s="27"/>
+      <c r="G50" s="27"/>
+      <c r="H50" s="27"/>
+      <c r="I50" s="27"/>
+      <c r="J50" s="21"/>
+      <c r="K50" s="22"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A51" s="52"/>
-      <c r="B51" s="52"/>
-      <c r="C51" s="52"/>
-      <c r="D51" s="52"/>
-      <c r="E51" s="52"/>
-      <c r="F51" s="52"/>
-      <c r="G51" s="53"/>
-      <c r="H51" s="53"/>
-      <c r="I51" s="53"/>
-      <c r="J51" s="45"/>
-      <c r="K51" s="48"/>
+      <c r="A51" s="28"/>
+      <c r="B51" s="28"/>
+      <c r="C51" s="28"/>
+      <c r="D51" s="28"/>
+      <c r="E51" s="28"/>
+      <c r="F51" s="28"/>
+      <c r="G51" s="29"/>
+      <c r="H51" s="29"/>
+      <c r="I51" s="29"/>
+      <c r="J51" s="21"/>
+      <c r="K51" s="24"/>
     </row>
     <row r="52" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A52" s="50"/>
-      <c r="B52" s="54"/>
-      <c r="C52" s="54"/>
-      <c r="D52" s="54"/>
-      <c r="E52" s="54"/>
-      <c r="F52" s="54"/>
-      <c r="G52" s="54"/>
-      <c r="H52" s="54"/>
-      <c r="I52" s="55"/>
-      <c r="J52" s="45"/>
-      <c r="K52" s="46"/>
+      <c r="A52" s="26"/>
+      <c r="B52" s="30"/>
+      <c r="C52" s="30"/>
+      <c r="D52" s="30"/>
+      <c r="E52" s="30"/>
+      <c r="F52" s="30"/>
+      <c r="G52" s="30"/>
+      <c r="H52" s="30"/>
+      <c r="I52" s="31"/>
+      <c r="J52" s="21"/>
+      <c r="K52" s="22"/>
     </row>
     <row r="53" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A53" s="50"/>
-      <c r="B53" s="54"/>
-      <c r="C53" s="54"/>
-      <c r="D53" s="54"/>
-      <c r="E53" s="54"/>
-      <c r="F53" s="54"/>
-      <c r="G53" s="54"/>
-      <c r="H53" s="54"/>
-      <c r="I53" s="55"/>
-      <c r="J53" s="45"/>
-      <c r="K53" s="46"/>
+      <c r="A53" s="26"/>
+      <c r="B53" s="30"/>
+      <c r="C53" s="30"/>
+      <c r="D53" s="30"/>
+      <c r="E53" s="30"/>
+      <c r="F53" s="30"/>
+      <c r="G53" s="30"/>
+      <c r="H53" s="30"/>
+      <c r="I53" s="31"/>
+      <c r="J53" s="21"/>
+      <c r="K53" s="22"/>
     </row>
     <row r="54" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A54" s="50"/>
-      <c r="B54" s="54"/>
-      <c r="C54" s="54"/>
-      <c r="D54" s="54"/>
-      <c r="E54" s="54"/>
-      <c r="F54" s="54"/>
-      <c r="G54" s="54"/>
-      <c r="H54" s="54"/>
-      <c r="I54" s="55"/>
-      <c r="J54" s="45"/>
-      <c r="K54" s="46"/>
+      <c r="A54" s="26"/>
+      <c r="B54" s="30"/>
+      <c r="C54" s="30"/>
+      <c r="D54" s="30"/>
+      <c r="E54" s="30"/>
+      <c r="F54" s="30"/>
+      <c r="G54" s="30"/>
+      <c r="H54" s="30"/>
+      <c r="I54" s="31"/>
+      <c r="J54" s="21"/>
+      <c r="K54" s="22"/>
     </row>
     <row r="55" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A55" s="50"/>
-      <c r="B55" s="54"/>
-      <c r="C55" s="54"/>
-      <c r="D55" s="54"/>
-      <c r="E55" s="54"/>
-      <c r="F55" s="54"/>
-      <c r="G55" s="54"/>
-      <c r="H55" s="54"/>
-      <c r="I55" s="55"/>
-      <c r="J55" s="45"/>
-      <c r="K55" s="46"/>
+      <c r="A55" s="26"/>
+      <c r="B55" s="30"/>
+      <c r="C55" s="30"/>
+      <c r="D55" s="30"/>
+      <c r="E55" s="30"/>
+      <c r="F55" s="30"/>
+      <c r="G55" s="30"/>
+      <c r="H55" s="30"/>
+      <c r="I55" s="31"/>
+      <c r="J55" s="21"/>
+      <c r="K55" s="22"/>
     </row>
     <row r="56" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A56" s="50"/>
-      <c r="B56" s="54"/>
-      <c r="C56" s="54"/>
-      <c r="D56" s="54"/>
-      <c r="E56" s="54"/>
-      <c r="F56" s="54"/>
-      <c r="G56" s="54"/>
-      <c r="H56" s="54"/>
-      <c r="I56" s="55"/>
-      <c r="J56" s="45"/>
-      <c r="K56" s="46"/>
+      <c r="A56" s="26"/>
+      <c r="B56" s="30"/>
+      <c r="C56" s="30"/>
+      <c r="D56" s="30"/>
+      <c r="E56" s="30"/>
+      <c r="F56" s="30"/>
+      <c r="G56" s="30"/>
+      <c r="H56" s="30"/>
+      <c r="I56" s="31"/>
+      <c r="J56" s="21"/>
+      <c r="K56" s="22"/>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A57" s="47"/>
-      <c r="B57" s="45"/>
-      <c r="C57" s="45"/>
-      <c r="D57" s="45"/>
-      <c r="E57" s="45"/>
-      <c r="F57" s="45"/>
-      <c r="G57" s="45"/>
-      <c r="H57" s="45"/>
-      <c r="I57" s="56"/>
-      <c r="J57" s="45"/>
-      <c r="K57" s="46"/>
+      <c r="A57" s="23"/>
+      <c r="B57" s="21"/>
+      <c r="C57" s="21"/>
+      <c r="D57" s="21"/>
+      <c r="E57" s="21"/>
+      <c r="F57" s="21"/>
+      <c r="G57" s="21"/>
+      <c r="H57" s="21"/>
+      <c r="I57" s="32"/>
+      <c r="J57" s="21"/>
+      <c r="K57" s="22"/>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A58" s="47"/>
-      <c r="B58" s="45"/>
-      <c r="C58" s="45"/>
-      <c r="D58" s="45"/>
-      <c r="E58" s="45"/>
-      <c r="F58" s="45"/>
-      <c r="G58" s="45"/>
-      <c r="H58" s="45"/>
-      <c r="I58" s="45"/>
-      <c r="J58" s="45"/>
-      <c r="K58" s="46"/>
+      <c r="A58" s="23"/>
+      <c r="B58" s="21"/>
+      <c r="C58" s="21"/>
+      <c r="D58" s="21"/>
+      <c r="E58" s="21"/>
+      <c r="F58" s="21"/>
+      <c r="G58" s="21"/>
+      <c r="H58" s="21"/>
+      <c r="I58" s="21"/>
+      <c r="J58" s="21"/>
+      <c r="K58" s="22"/>
     </row>
     <row r="59" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A59" s="47"/>
-      <c r="B59" s="45"/>
-      <c r="C59" s="45"/>
-      <c r="D59" s="45"/>
-      <c r="E59" s="45"/>
-      <c r="F59" s="45"/>
-      <c r="G59" s="45"/>
-      <c r="H59" s="45"/>
-      <c r="I59" s="45"/>
-      <c r="J59" s="45"/>
-      <c r="K59" s="46"/>
+      <c r="A59" s="23"/>
+      <c r="B59" s="21"/>
+      <c r="C59" s="21"/>
+      <c r="D59" s="21"/>
+      <c r="E59" s="21"/>
+      <c r="F59" s="21"/>
+      <c r="G59" s="21"/>
+      <c r="H59" s="21"/>
+      <c r="I59" s="21"/>
+      <c r="J59" s="21"/>
+      <c r="K59" s="22"/>
     </row>
     <row r="60" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A60" s="50"/>
-      <c r="B60" s="51"/>
-      <c r="C60" s="51"/>
-      <c r="D60" s="51"/>
-      <c r="E60" s="51"/>
-      <c r="F60" s="51"/>
-      <c r="G60" s="51"/>
-      <c r="H60" s="51"/>
-      <c r="I60" s="51"/>
-      <c r="J60" s="45"/>
-      <c r="K60" s="46"/>
+      <c r="A60" s="26"/>
+      <c r="B60" s="27"/>
+      <c r="C60" s="27"/>
+      <c r="D60" s="27"/>
+      <c r="E60" s="27"/>
+      <c r="F60" s="27"/>
+      <c r="G60" s="27"/>
+      <c r="H60" s="27"/>
+      <c r="I60" s="27"/>
+      <c r="J60" s="21"/>
+      <c r="K60" s="22"/>
     </row>
     <row r="61" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A61" s="52"/>
-      <c r="B61" s="52"/>
-      <c r="C61" s="52"/>
-      <c r="D61" s="52"/>
-      <c r="E61" s="52"/>
-      <c r="F61" s="52"/>
-      <c r="G61" s="53"/>
-      <c r="H61" s="53"/>
-      <c r="I61" s="53"/>
-      <c r="J61" s="45"/>
-      <c r="K61" s="48"/>
+      <c r="A61" s="28"/>
+      <c r="B61" s="28"/>
+      <c r="C61" s="28"/>
+      <c r="D61" s="28"/>
+      <c r="E61" s="28"/>
+      <c r="F61" s="28"/>
+      <c r="G61" s="29"/>
+      <c r="H61" s="29"/>
+      <c r="I61" s="29"/>
+      <c r="J61" s="21"/>
+      <c r="K61" s="24"/>
     </row>
     <row r="62" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A62" s="50"/>
-      <c r="B62" s="54"/>
-      <c r="C62" s="54"/>
-      <c r="D62" s="54"/>
-      <c r="E62" s="54"/>
-      <c r="F62" s="54"/>
-      <c r="G62" s="54"/>
-      <c r="H62" s="54"/>
-      <c r="I62" s="55"/>
-      <c r="J62" s="45"/>
-      <c r="K62" s="46"/>
+      <c r="A62" s="26"/>
+      <c r="B62" s="30"/>
+      <c r="C62" s="30"/>
+      <c r="D62" s="30"/>
+      <c r="E62" s="30"/>
+      <c r="F62" s="30"/>
+      <c r="G62" s="30"/>
+      <c r="H62" s="30"/>
+      <c r="I62" s="31"/>
+      <c r="J62" s="21"/>
+      <c r="K62" s="22"/>
     </row>
     <row r="63" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A63" s="50"/>
-      <c r="B63" s="54"/>
-      <c r="C63" s="54"/>
-      <c r="D63" s="54"/>
-      <c r="E63" s="54"/>
-      <c r="F63" s="54"/>
-      <c r="G63" s="54"/>
-      <c r="H63" s="54"/>
-      <c r="I63" s="55"/>
-      <c r="J63" s="45"/>
-      <c r="K63" s="46"/>
+      <c r="A63" s="26"/>
+      <c r="B63" s="30"/>
+      <c r="C63" s="30"/>
+      <c r="D63" s="30"/>
+      <c r="E63" s="30"/>
+      <c r="F63" s="30"/>
+      <c r="G63" s="30"/>
+      <c r="H63" s="30"/>
+      <c r="I63" s="31"/>
+      <c r="J63" s="21"/>
+      <c r="K63" s="22"/>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A64" s="50"/>
-      <c r="B64" s="54"/>
-      <c r="C64" s="54"/>
-      <c r="D64" s="54"/>
-      <c r="E64" s="54"/>
-      <c r="F64" s="54"/>
-      <c r="G64" s="54"/>
-      <c r="H64" s="54"/>
-      <c r="I64" s="55"/>
-      <c r="J64" s="45"/>
-      <c r="K64" s="46"/>
+      <c r="A64" s="26"/>
+      <c r="B64" s="30"/>
+      <c r="C64" s="30"/>
+      <c r="D64" s="30"/>
+      <c r="E64" s="30"/>
+      <c r="F64" s="30"/>
+      <c r="G64" s="30"/>
+      <c r="H64" s="30"/>
+      <c r="I64" s="31"/>
+      <c r="J64" s="21"/>
+      <c r="K64" s="22"/>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A65" s="50"/>
-      <c r="B65" s="54"/>
-      <c r="C65" s="54"/>
-      <c r="D65" s="54"/>
-      <c r="E65" s="54"/>
-      <c r="F65" s="54"/>
-      <c r="G65" s="54"/>
-      <c r="H65" s="54"/>
-      <c r="I65" s="55"/>
-      <c r="J65" s="45"/>
-      <c r="K65" s="46"/>
+      <c r="A65" s="26"/>
+      <c r="B65" s="30"/>
+      <c r="C65" s="30"/>
+      <c r="D65" s="30"/>
+      <c r="E65" s="30"/>
+      <c r="F65" s="30"/>
+      <c r="G65" s="30"/>
+      <c r="H65" s="30"/>
+      <c r="I65" s="31"/>
+      <c r="J65" s="21"/>
+      <c r="K65" s="22"/>
     </row>
     <row r="66" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A66" s="50"/>
-      <c r="B66" s="54"/>
-      <c r="C66" s="54"/>
-      <c r="D66" s="54"/>
-      <c r="E66" s="54"/>
-      <c r="F66" s="54"/>
-      <c r="G66" s="54"/>
-      <c r="H66" s="54"/>
-      <c r="I66" s="55"/>
-      <c r="J66" s="45"/>
-      <c r="K66" s="46"/>
+      <c r="A66" s="26"/>
+      <c r="B66" s="30"/>
+      <c r="C66" s="30"/>
+      <c r="D66" s="30"/>
+      <c r="E66" s="30"/>
+      <c r="F66" s="30"/>
+      <c r="G66" s="30"/>
+      <c r="H66" s="30"/>
+      <c r="I66" s="31"/>
+      <c r="J66" s="21"/>
+      <c r="K66" s="22"/>
     </row>
     <row r="67" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A67" s="47"/>
-      <c r="B67" s="45"/>
-      <c r="C67" s="45"/>
-      <c r="D67" s="45"/>
-      <c r="E67" s="45"/>
-      <c r="F67" s="45"/>
-      <c r="G67" s="45"/>
-      <c r="H67" s="45"/>
-      <c r="I67" s="56"/>
-      <c r="J67" s="45"/>
-      <c r="K67" s="46"/>
+      <c r="A67" s="23"/>
+      <c r="B67" s="21"/>
+      <c r="C67" s="21"/>
+      <c r="D67" s="21"/>
+      <c r="E67" s="21"/>
+      <c r="F67" s="21"/>
+      <c r="G67" s="21"/>
+      <c r="H67" s="21"/>
+      <c r="I67" s="32"/>
+      <c r="J67" s="21"/>
+      <c r="K67" s="22"/>
     </row>
     <row r="68" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A68" s="47"/>
-      <c r="B68" s="45"/>
-      <c r="C68" s="45"/>
-      <c r="D68" s="45"/>
-      <c r="E68" s="45"/>
-      <c r="F68" s="45"/>
-      <c r="G68" s="45"/>
-      <c r="H68" s="45"/>
-      <c r="I68" s="45"/>
-      <c r="J68" s="45"/>
-      <c r="K68" s="46"/>
+      <c r="A68" s="23"/>
+      <c r="B68" s="21"/>
+      <c r="C68" s="21"/>
+      <c r="D68" s="21"/>
+      <c r="E68" s="21"/>
+      <c r="F68" s="21"/>
+      <c r="G68" s="21"/>
+      <c r="H68" s="21"/>
+      <c r="I68" s="21"/>
+      <c r="J68" s="21"/>
+      <c r="K68" s="22"/>
     </row>
     <row r="69" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A69" s="47"/>
-      <c r="B69" s="45"/>
-      <c r="C69" s="45"/>
-      <c r="D69" s="45"/>
-      <c r="E69" s="45"/>
-      <c r="F69" s="45"/>
-      <c r="G69" s="45"/>
-      <c r="H69" s="45"/>
-      <c r="I69" s="45"/>
-      <c r="J69" s="45"/>
-      <c r="K69" s="46"/>
+      <c r="A69" s="23"/>
+      <c r="B69" s="21"/>
+      <c r="C69" s="21"/>
+      <c r="D69" s="21"/>
+      <c r="E69" s="21"/>
+      <c r="F69" s="21"/>
+      <c r="G69" s="21"/>
+      <c r="H69" s="21"/>
+      <c r="I69" s="21"/>
+      <c r="J69" s="21"/>
+      <c r="K69" s="22"/>
     </row>
     <row r="70" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A70" s="50"/>
-      <c r="B70" s="51"/>
-      <c r="C70" s="51"/>
-      <c r="D70" s="51"/>
-      <c r="E70" s="51"/>
-      <c r="F70" s="51"/>
-      <c r="G70" s="51"/>
-      <c r="H70" s="51"/>
-      <c r="I70" s="51"/>
-      <c r="J70" s="45"/>
-      <c r="K70" s="46"/>
+      <c r="A70" s="26"/>
+      <c r="B70" s="27"/>
+      <c r="C70" s="27"/>
+      <c r="D70" s="27"/>
+      <c r="E70" s="27"/>
+      <c r="F70" s="27"/>
+      <c r="G70" s="27"/>
+      <c r="H70" s="27"/>
+      <c r="I70" s="27"/>
+      <c r="J70" s="21"/>
+      <c r="K70" s="22"/>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A71" s="52"/>
-      <c r="B71" s="52"/>
-      <c r="C71" s="52"/>
-      <c r="D71" s="52"/>
-      <c r="E71" s="52"/>
-      <c r="F71" s="52"/>
-      <c r="G71" s="53"/>
-      <c r="H71" s="53"/>
-      <c r="I71" s="53"/>
-      <c r="J71" s="45"/>
-      <c r="K71" s="48"/>
+      <c r="A71" s="28"/>
+      <c r="B71" s="28"/>
+      <c r="C71" s="28"/>
+      <c r="D71" s="28"/>
+      <c r="E71" s="28"/>
+      <c r="F71" s="28"/>
+      <c r="G71" s="29"/>
+      <c r="H71" s="29"/>
+      <c r="I71" s="29"/>
+      <c r="J71" s="21"/>
+      <c r="K71" s="24"/>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A72" s="50"/>
-      <c r="B72" s="54"/>
-      <c r="C72" s="54"/>
-      <c r="D72" s="54"/>
-      <c r="E72" s="54"/>
-      <c r="F72" s="54"/>
-      <c r="G72" s="54"/>
-      <c r="H72" s="54"/>
-      <c r="I72" s="55"/>
-      <c r="J72" s="45"/>
-      <c r="K72" s="46"/>
+      <c r="A72" s="26"/>
+      <c r="B72" s="30"/>
+      <c r="C72" s="30"/>
+      <c r="D72" s="30"/>
+      <c r="E72" s="30"/>
+      <c r="F72" s="30"/>
+      <c r="G72" s="30"/>
+      <c r="H72" s="30"/>
+      <c r="I72" s="31"/>
+      <c r="J72" s="21"/>
+      <c r="K72" s="22"/>
     </row>
     <row r="73" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A73" s="50"/>
-      <c r="B73" s="54"/>
-      <c r="C73" s="54"/>
-      <c r="D73" s="54"/>
-      <c r="E73" s="54"/>
-      <c r="F73" s="54"/>
-      <c r="G73" s="54"/>
-      <c r="H73" s="54"/>
-      <c r="I73" s="55"/>
-      <c r="J73" s="45"/>
-      <c r="K73" s="46"/>
+      <c r="A73" s="26"/>
+      <c r="B73" s="30"/>
+      <c r="C73" s="30"/>
+      <c r="D73" s="30"/>
+      <c r="E73" s="30"/>
+      <c r="F73" s="30"/>
+      <c r="G73" s="30"/>
+      <c r="H73" s="30"/>
+      <c r="I73" s="31"/>
+      <c r="J73" s="21"/>
+      <c r="K73" s="22"/>
     </row>
     <row r="74" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A74" s="50"/>
-      <c r="B74" s="54"/>
-      <c r="C74" s="54"/>
-      <c r="D74" s="54"/>
-      <c r="E74" s="54"/>
-      <c r="F74" s="54"/>
-      <c r="G74" s="54"/>
-      <c r="H74" s="54"/>
-      <c r="I74" s="55"/>
-      <c r="J74" s="45"/>
-      <c r="K74" s="46"/>
+      <c r="A74" s="26"/>
+      <c r="B74" s="30"/>
+      <c r="C74" s="30"/>
+      <c r="D74" s="30"/>
+      <c r="E74" s="30"/>
+      <c r="F74" s="30"/>
+      <c r="G74" s="30"/>
+      <c r="H74" s="30"/>
+      <c r="I74" s="31"/>
+      <c r="J74" s="21"/>
+      <c r="K74" s="22"/>
     </row>
     <row r="75" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A75" s="50"/>
-      <c r="B75" s="54"/>
-      <c r="C75" s="54"/>
-      <c r="D75" s="54"/>
-      <c r="E75" s="54"/>
-      <c r="F75" s="54"/>
-      <c r="G75" s="54"/>
-      <c r="H75" s="54"/>
-      <c r="I75" s="55"/>
-      <c r="J75" s="45"/>
-      <c r="K75" s="46"/>
+      <c r="A75" s="26"/>
+      <c r="B75" s="30"/>
+      <c r="C75" s="30"/>
+      <c r="D75" s="30"/>
+      <c r="E75" s="30"/>
+      <c r="F75" s="30"/>
+      <c r="G75" s="30"/>
+      <c r="H75" s="30"/>
+      <c r="I75" s="31"/>
+      <c r="J75" s="21"/>
+      <c r="K75" s="22"/>
     </row>
     <row r="76" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A76" s="50"/>
-      <c r="B76" s="54"/>
-      <c r="C76" s="54"/>
-      <c r="D76" s="54"/>
-      <c r="E76" s="54"/>
-      <c r="F76" s="54"/>
-      <c r="G76" s="54"/>
-      <c r="H76" s="54"/>
-      <c r="I76" s="55"/>
-      <c r="J76" s="45"/>
-      <c r="K76" s="46"/>
+      <c r="A76" s="26"/>
+      <c r="B76" s="30"/>
+      <c r="C76" s="30"/>
+      <c r="D76" s="30"/>
+      <c r="E76" s="30"/>
+      <c r="F76" s="30"/>
+      <c r="G76" s="30"/>
+      <c r="H76" s="30"/>
+      <c r="I76" s="31"/>
+      <c r="J76" s="21"/>
+      <c r="K76" s="22"/>
     </row>
     <row r="77" spans="1:11" x14ac:dyDescent="0.45">
-      <c r="A77" s="47"/>
-      <c r="B77" s="45"/>
-      <c r="C77" s="45"/>
-      <c r="D77" s="45"/>
-      <c r="E77" s="45"/>
-      <c r="F77" s="45"/>
-      <c r="G77" s="45"/>
-      <c r="H77" s="45"/>
-      <c r="I77" s="56"/>
-      <c r="J77" s="45"/>
-      <c r="K77" s="46"/>
+      <c r="A77" s="23"/>
+      <c r="B77" s="21"/>
+      <c r="C77" s="21"/>
+      <c r="D77" s="21"/>
+      <c r="E77" s="21"/>
+      <c r="F77" s="21"/>
+      <c r="G77" s="21"/>
+      <c r="H77" s="21"/>
+      <c r="I77" s="32"/>
+      <c r="J77" s="21"/>
+      <c r="K77" s="22"/>
     </row>
   </sheetData>
   <phoneticPr fontId="5" type="noConversion"/>
@@ -11916,7 +11997,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59EEF642-6DF7-074B-8B4B-EA7E7E078885}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A184" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A163" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="P128" sqref="P128"/>
     </sheetView>
   </sheetViews>

</xml_diff>